<commit_message>
added Input registers handler
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Range</t>
   </si>
@@ -33,13 +33,127 @@
   </si>
   <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>0-31</t>
+  </si>
+  <si>
+    <t>32-63</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Analog inputs</t>
+  </si>
+  <si>
+    <t>64-95</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Counters</t>
+  </si>
+  <si>
+    <t>Digital Inputs</t>
+  </si>
+  <si>
+    <t>96-127</t>
+  </si>
+  <si>
+    <t>128-159</t>
+  </si>
+  <si>
+    <t>Digital inputs</t>
+  </si>
+  <si>
+    <t>Holding</t>
+  </si>
+  <si>
+    <t>Digital outputs</t>
+  </si>
+  <si>
+    <t>Analog outputs</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Analog input 0</t>
+  </si>
+  <si>
+    <t>Analog input 1</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>64, 65</t>
+  </si>
+  <si>
+    <t>Counter 0</t>
+  </si>
+  <si>
+    <t>Reg. Address</t>
+  </si>
+  <si>
+    <t>66, 67</t>
+  </si>
+  <si>
+    <t>Counter 1</t>
+  </si>
+  <si>
+    <t>92, 93</t>
+  </si>
+  <si>
+    <t>160-192</t>
+  </si>
+  <si>
+    <t>Counter 14</t>
+  </si>
+  <si>
+    <t>Analog Output 0</t>
+  </si>
+  <si>
+    <t>Analog Output 1</t>
+  </si>
+  <si>
+    <t>Analog Output 2</t>
+  </si>
+  <si>
+    <t>Analog Output 3</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Write)</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Set)</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Clear)</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Toggle)</t>
+  </si>
+  <si>
+    <t>Analog Input 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,16 +162,55 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -65,12 +218,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -351,30 +587,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E3"/>
+  <dimension ref="C2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="8">
+        <v>32</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="8">
+        <v>33</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="8">
+        <v>42</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="10">
+        <v>96</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="14">
+        <v>128</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I14" s="14">
+        <v>129</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="14">
+        <v>130</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="14">
+        <v>131</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="12">
+        <v>160</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="12">
+        <v>161</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="12">
+        <v>162</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="12">
+        <v>163</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
regmap table minor fix
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Range</t>
   </si>
@@ -134,19 +134,22 @@
     <t>Analog Output 3</t>
   </si>
   <si>
-    <t>Digital Outputs (Write)</t>
-  </si>
-  <si>
-    <t>Digital Outputs (Set)</t>
-  </si>
-  <si>
-    <t>Digital Outputs (Clear)</t>
-  </si>
-  <si>
-    <t>Digital Outputs (Toggle)</t>
-  </si>
-  <si>
     <t>Analog Input 10</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Read/Write)</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Set)*</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Clear)*</t>
+  </si>
+  <si>
+    <t>Digital Outputs (Toggle)*</t>
+  </si>
+  <si>
+    <t>* - write only</t>
   </si>
 </sst>
 </file>
@@ -274,19 +277,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -307,6 +301,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -587,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J20"/>
+  <dimension ref="C2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,18 +606,19 @@
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="I2" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="I2" s="16" t="s">
         <v>19</v>
       </c>
+      <c r="J2" s="16"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -622,10 +630,10 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -639,10 +647,10 @@
       <c r="E4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="5">
         <v>32</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -656,10 +664,10 @@
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="5">
         <v>33</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -673,10 +681,10 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -690,11 +698,11 @@
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="5">
         <v>42</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>40</v>
+      <c r="J7" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
@@ -707,10 +715,10 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -724,104 +732,110 @@
       <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <v>96</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I13" s="14">
+      <c r="I13" s="11">
         <v>128</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I14" s="14">
+      <c r="I14" s="11">
         <v>129</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I15" s="14">
+      <c r="I15" s="11">
         <v>130</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="12" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="14">
+      <c r="I16" s="11">
         <v>131</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="12">
+      <c r="I17" s="9">
         <v>160</v>
       </c>
-      <c r="J17" s="13" t="s">
-        <v>36</v>
+      <c r="J17" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="12">
+      <c r="I18" s="9">
         <v>161</v>
       </c>
-      <c r="J18" s="13" t="s">
-        <v>37</v>
+      <c r="J18" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="12">
+      <c r="I19" s="9">
         <v>162</v>
       </c>
-      <c r="J19" s="13" t="s">
-        <v>38</v>
+      <c r="J19" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="12">
+      <c r="I20" s="9">
         <v>163</v>
       </c>
-      <c r="J20" s="13" t="s">
-        <v>39</v>
+      <c r="J20" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added getting uptime to the modbus and shell interfaces
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\iomodule-firm\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ChibiOS_based\iomodule\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Range</t>
   </si>
@@ -116,9 +116,6 @@
     <t>92, 93</t>
   </si>
   <si>
-    <t>160-192</t>
-  </si>
-  <si>
     <t>Counter 14</t>
   </si>
   <si>
@@ -150,6 +147,21 @@
   </si>
   <si>
     <t>* - write only</t>
+  </si>
+  <si>
+    <t>160-191</t>
+  </si>
+  <si>
+    <t>192-223</t>
+  </si>
+  <si>
+    <t>System stats</t>
+  </si>
+  <si>
+    <t>System uptime</t>
+  </si>
+  <si>
+    <t>192, 193</t>
   </si>
 </sst>
 </file>
@@ -175,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +224,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -277,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -301,6 +319,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,7 +332,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -594,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J22"/>
+  <dimension ref="C2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,15 +637,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
-      <c r="I2" s="16" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="I2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="16"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -702,7 +729,7 @@
         <v>42</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
@@ -724,7 +751,7 @@
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>16</v>
@@ -740,6 +767,15 @@
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>43</v>
+      </c>
       <c r="I10" s="6" t="s">
         <v>23</v>
       </c>
@@ -752,7 +788,7 @@
         <v>29</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
@@ -768,7 +804,7 @@
         <v>128</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
@@ -776,7 +812,7 @@
         <v>129</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
@@ -784,7 +820,7 @@
         <v>130</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
@@ -792,7 +828,7 @@
         <v>131</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="9:10" x14ac:dyDescent="0.25">
@@ -800,7 +836,7 @@
         <v>160</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
@@ -808,7 +844,7 @@
         <v>161</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="9:10" x14ac:dyDescent="0.25">
@@ -816,7 +852,7 @@
         <v>162</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
@@ -824,12 +860,24 @@
         <v>163</v>
       </c>
       <c r="J20" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="13" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="J22" s="17" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some registers to regmap
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
   <si>
     <t>Range</t>
   </si>
@@ -209,15 +209,9 @@
     <t>400-499</t>
   </si>
   <si>
-    <t>300-399</t>
-  </si>
-  <si>
     <t>1-wire raw data</t>
   </si>
   <si>
-    <t>temperature control</t>
-  </si>
-  <si>
     <t>Temperature</t>
   </si>
   <si>
@@ -252,6 +246,21 @@
   </si>
   <si>
     <t>490-496</t>
+  </si>
+  <si>
+    <t>1-Wire and temperature control registers</t>
+  </si>
+  <si>
+    <t>350-361</t>
+  </si>
+  <si>
+    <t>temperature control setup</t>
+  </si>
+  <si>
+    <t>temperature control status</t>
+  </si>
+  <si>
+    <t>300-339</t>
   </si>
 </sst>
 </file>
@@ -339,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -399,11 +408,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -437,11 +526,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,10 +542,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -744,17 +857,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M42"/>
+  <dimension ref="C2:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="2.21875" customWidth="1"/>
+    <col min="2" max="2" width="2.44140625" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" customWidth="1"/>
+    <col min="7" max="7" width="2.109375" customWidth="1"/>
+    <col min="8" max="8" width="2.77734375" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="27.88671875" customWidth="1"/>
     <col min="11" max="11" width="7.44140625" customWidth="1"/>
@@ -762,15 +880,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-      <c r="I2" s="25" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="I2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="25"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
@@ -910,13 +1028,13 @@
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>29</v>
@@ -927,13 +1045,13 @@
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="I12" s="7">
         <v>96</v>
@@ -944,13 +1062,13 @@
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="I13" s="11">
         <v>128</v>
@@ -960,6 +1078,15 @@
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="I14" s="11">
         <v>129</v>
       </c>
@@ -1024,22 +1151,22 @@
       </c>
     </row>
     <row r="22" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I22" s="26">
+      <c r="I22" s="19">
         <v>250</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I23" s="19">
+        <v>251</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="K23" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I23" s="26">
-        <v>251</v>
-      </c>
-      <c r="J23" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="K23" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="24" spans="9:13" x14ac:dyDescent="0.3">
@@ -1052,219 +1179,279 @@
       </c>
     </row>
     <row r="26" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="K26" t="s">
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I27" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="43"/>
+    </row>
+    <row r="28" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="K28" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I27" s="19">
+    <row r="29" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I29" s="25">
         <v>300</v>
       </c>
-      <c r="J27" s="19" t="s">
+      <c r="J29" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="K27" s="19">
+      <c r="K29" s="26">
         <v>4</v>
       </c>
-      <c r="L27" s="19" t="s">
+      <c r="L29" s="27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I28" s="19">
+    <row r="30" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I30" s="28">
         <v>304</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J30" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="K28" s="19">
+      <c r="K30" s="29">
         <v>4</v>
       </c>
-      <c r="L28" s="19" t="s">
+      <c r="L30" s="30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I29" s="19">
+    <row r="31" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I31" s="28">
         <v>308</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J31" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K31" s="29">
         <v>1</v>
       </c>
-      <c r="L29" s="19" t="s">
+      <c r="L31" s="30" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I30" s="19">
+      <c r="M31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I32" s="28">
         <v>309</v>
       </c>
-      <c r="J30" s="19" t="s">
+      <c r="J32" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K32" s="29">
         <v>1</v>
       </c>
-      <c r="L30" s="19" t="s">
+      <c r="L32" s="30" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="31" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I31" s="19">
+      <c r="M32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I33" s="31">
         <v>310</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="J33" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="K33" s="32">
+        <v>10</v>
+      </c>
+      <c r="L33" s="33"/>
+    </row>
+    <row r="34" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I34" s="31">
+        <v>320</v>
+      </c>
+      <c r="J34" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="K34" s="32">
+        <v>10</v>
+      </c>
+      <c r="L34" s="33"/>
+    </row>
+    <row r="35" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I35" s="34">
+        <v>330</v>
+      </c>
+      <c r="J35" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="K35" s="35">
+        <v>10</v>
+      </c>
+      <c r="L35" s="36"/>
+    </row>
+    <row r="37" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I37" s="25">
+        <v>350</v>
+      </c>
+      <c r="J37" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K37" s="26">
         <v>1</v>
       </c>
-      <c r="L31" s="19" t="s">
+      <c r="L37" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M37" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I32" s="19">
-        <v>311</v>
-      </c>
-      <c r="J32" s="19" t="s">
+    <row r="38" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I38" s="28">
+        <v>351</v>
+      </c>
+      <c r="J38" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K38" s="29">
         <v>1</v>
       </c>
-      <c r="L32" s="19" t="s">
+      <c r="L38" s="30" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="33" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I33" s="19">
-        <v>312</v>
-      </c>
-      <c r="J33" s="19" t="s">
+      <c r="M38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I39" s="28">
+        <v>352</v>
+      </c>
+      <c r="J39" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="K33" s="19">
+      <c r="K39" s="29">
         <v>1</v>
       </c>
-      <c r="L33" s="19" t="s">
+      <c r="L39" s="30" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I34" s="20">
-        <v>313</v>
-      </c>
-      <c r="J34" s="20" t="s">
+      <c r="M39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I40" s="31">
+        <v>353</v>
+      </c>
+      <c r="J40" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="K34" s="20">
-        <v>13</v>
-      </c>
-      <c r="L34" s="20"/>
-    </row>
-    <row r="35" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I35" s="20">
-        <v>326</v>
-      </c>
-      <c r="J35" s="20" t="s">
+      <c r="K40" s="32">
+        <v>3</v>
+      </c>
+      <c r="L40" s="33"/>
+    </row>
+    <row r="41" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I41" s="31">
+        <v>356</v>
+      </c>
+      <c r="J41" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="K35" s="20">
-        <v>13</v>
-      </c>
-      <c r="L35" s="20"/>
-    </row>
-    <row r="36" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I36" s="20">
-        <v>339</v>
-      </c>
-      <c r="J36" s="20" t="s">
+      <c r="K41" s="32">
+        <v>3</v>
+      </c>
+      <c r="L41" s="33"/>
+    </row>
+    <row r="42" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I42" s="34">
+        <v>359</v>
+      </c>
+      <c r="J42" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="K36" s="20">
-        <v>13</v>
-      </c>
-      <c r="L36" s="20"/>
-    </row>
-    <row r="38" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I38" s="19">
+      <c r="K42" s="35">
+        <v>3</v>
+      </c>
+      <c r="L42" s="36"/>
+    </row>
+    <row r="44" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I44" s="25">
         <v>400</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J44" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="K44" s="26">
+        <v>4</v>
+      </c>
+      <c r="L44" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I45" s="28">
+        <v>404</v>
+      </c>
+      <c r="J45" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="K45" s="29">
+        <v>1</v>
+      </c>
+      <c r="L45" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="M45" t="s">
         <v>67</v>
       </c>
-      <c r="K38" s="19">
-        <v>4</v>
-      </c>
-      <c r="L38" s="19" t="s">
+    </row>
+    <row r="46" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I46" s="28">
+        <v>405</v>
+      </c>
+      <c r="J46" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" s="29">
+        <v>1</v>
+      </c>
+      <c r="L46" s="30" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="39" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I39" s="19">
-        <v>404</v>
-      </c>
-      <c r="J39" s="19" t="s">
+      <c r="M46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I47" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="K39" s="19">
-        <v>1</v>
-      </c>
-      <c r="L39" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="M39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I40" s="19">
-        <v>405</v>
-      </c>
-      <c r="J40" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="K40" s="19">
-        <v>1</v>
-      </c>
-      <c r="L40" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="M40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I41" s="21" t="s">
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="30"/>
+    </row>
+    <row r="48" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I48" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="J48" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-    </row>
-    <row r="42" spans="9:13" x14ac:dyDescent="0.3">
-      <c r="I42" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="J42" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="K42" s="19">
+      <c r="K48" s="39">
         <v>6</v>
       </c>
-      <c r="L42" s="19"/>
+      <c r="L48" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add status bits to doc
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
   <si>
     <t>Range</t>
   </si>
@@ -203,9 +203,6 @@
     <t>registers (x2bytes)</t>
   </si>
   <si>
-    <t>b0: channel on/off, b1: sensor1 on/off, b2: sensor2 on/off</t>
-  </si>
-  <si>
     <t>400-499</t>
   </si>
   <si>
@@ -261,6 +258,42 @@
   </si>
   <si>
     <t>300-339</t>
+  </si>
+  <si>
+    <t>channel setup t1 OK</t>
+  </si>
+  <si>
+    <t>channel setup t2 OK</t>
+  </si>
+  <si>
+    <t>long loop control needs heating</t>
+  </si>
+  <si>
+    <t>short loop control needs heating</t>
+  </si>
+  <si>
+    <t>long loop is overheated</t>
+  </si>
+  <si>
+    <t>short loop is overheated</t>
+  </si>
+  <si>
+    <t>control result. 1 = heating</t>
+  </si>
+  <si>
+    <t>temperature 1 (short loop) OK</t>
+  </si>
+  <si>
+    <t>temperature 2 (long loop) OK</t>
+  </si>
+  <si>
+    <t>safety check error. Heating off</t>
+  </si>
+  <si>
+    <t>look at channel status bits</t>
+  </si>
+  <si>
+    <t>channel status bits:</t>
   </si>
 </sst>
 </file>
@@ -492,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -569,6 +602,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -859,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,13 +1076,13 @@
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>29</v>
@@ -1045,13 +1093,13 @@
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I12" s="7">
         <v>96</v>
@@ -1062,13 +1110,13 @@
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I13" s="11">
         <v>128</v>
@@ -1079,13 +1127,13 @@
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I14" s="11">
         <v>129</v>
@@ -1110,7 +1158,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I17" s="9">
         <v>160</v>
       </c>
@@ -1118,7 +1166,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I18" s="9">
         <v>161</v>
       </c>
@@ -1126,7 +1174,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I19" s="9">
         <v>162</v>
       </c>
@@ -1134,7 +1182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I20" s="9">
         <v>163</v>
       </c>
@@ -1142,7 +1190,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I21" s="15" t="s">
         <v>45</v>
       </c>
@@ -1150,51 +1198,56 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I22" s="19">
         <v>250</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="9:13" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I23" s="19">
         <v>251</v>
       </c>
       <c r="J23" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" t="s">
         <v>69</v>
       </c>
-      <c r="K23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="9:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I24" s="17"/>
       <c r="J24" s="18"/>
     </row>
-    <row r="25" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
       <c r="J25" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
       <c r="J26" s="13"/>
     </row>
-    <row r="27" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I27" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J27" s="42"/>
       <c r="K27" s="42"/>
       <c r="L27" s="43"/>
     </row>
-    <row r="28" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
       <c r="K28" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C29" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="51"/>
+      <c r="E29" s="52"/>
       <c r="I29" s="25">
         <v>300</v>
       </c>
@@ -1208,7 +1261,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C30" s="44">
+        <v>0</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="46"/>
       <c r="I30" s="28">
         <v>304</v>
       </c>
@@ -1222,7 +1282,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C31" s="44">
+        <v>1</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="46"/>
       <c r="I31" s="28">
         <v>308</v>
       </c>
@@ -1236,10 +1303,17 @@
         <v>53</v>
       </c>
       <c r="M31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="9:13" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C32" s="44">
+        <v>2</v>
+      </c>
+      <c r="D32" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="46"/>
       <c r="I32" s="28">
         <v>309</v>
       </c>
@@ -1253,10 +1327,17 @@
         <v>53</v>
       </c>
       <c r="M32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="9:13" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C33" s="44">
+        <v>3</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="46"/>
       <c r="I33" s="31">
         <v>310</v>
       </c>
@@ -1268,7 +1349,14 @@
       </c>
       <c r="L33" s="33"/>
     </row>
-    <row r="34" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C34" s="44">
+        <v>4</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="46"/>
       <c r="I34" s="31">
         <v>320</v>
       </c>
@@ -1280,7 +1368,14 @@
       </c>
       <c r="L34" s="33"/>
     </row>
-    <row r="35" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C35" s="44">
+        <v>5</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" s="46"/>
       <c r="I35" s="34">
         <v>330</v>
       </c>
@@ -1292,7 +1387,23 @@
       </c>
       <c r="L35" s="36"/>
     </row>
-    <row r="37" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C36" s="44">
+        <v>6</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="46"/>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C37" s="44">
+        <v>7</v>
+      </c>
+      <c r="D37" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="46"/>
       <c r="I37" s="25">
         <v>350</v>
       </c>
@@ -1306,10 +1417,17 @@
         <v>52</v>
       </c>
       <c r="M37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="9:13" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C38" s="44">
+        <v>8</v>
+      </c>
+      <c r="D38" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="46"/>
       <c r="I38" s="28">
         <v>351</v>
       </c>
@@ -1323,10 +1441,17 @@
         <v>52</v>
       </c>
       <c r="M38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="9:13" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C39" s="47">
+        <v>9</v>
+      </c>
+      <c r="D39" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="49"/>
       <c r="I39" s="28">
         <v>352</v>
       </c>
@@ -1340,10 +1465,10 @@
         <v>52</v>
       </c>
       <c r="M39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="9:13" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I40" s="31">
         <v>353</v>
       </c>
@@ -1355,7 +1480,7 @@
       </c>
       <c r="L40" s="33"/>
     </row>
-    <row r="41" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I41" s="31">
         <v>356</v>
       </c>
@@ -1367,7 +1492,7 @@
       </c>
       <c r="L41" s="33"/>
     </row>
-    <row r="42" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I42" s="34">
         <v>359</v>
       </c>
@@ -1379,12 +1504,12 @@
       </c>
       <c r="L42" s="36"/>
     </row>
-    <row r="44" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I44" s="25">
         <v>400</v>
       </c>
       <c r="J44" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K44" s="26">
         <v>4</v>
@@ -1393,12 +1518,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I45" s="28">
         <v>404</v>
       </c>
       <c r="J45" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K45" s="29">
         <v>1</v>
@@ -1407,15 +1532,15 @@
         <v>52</v>
       </c>
       <c r="M45" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="9:13" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I46" s="28">
         <v>405</v>
       </c>
       <c r="J46" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K46" s="29">
         <v>1</v>
@@ -1424,23 +1549,23 @@
         <v>52</v>
       </c>
       <c r="M46" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="9:13" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I47" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J47" s="29"/>
       <c r="K47" s="29"/>
       <c r="L47" s="30"/>
     </row>
-    <row r="48" spans="9:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:13" x14ac:dyDescent="0.3">
       <c r="I48" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J48" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K48" s="39">
         <v>6</v>
@@ -1448,10 +1573,11 @@
       <c r="L48" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I27:L27"/>
+    <mergeCell ref="C29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
temp sontrol works with eeprom and eeprom page size set
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Range</t>
   </si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>channel status bits:</t>
+  </si>
+  <si>
+    <t>Holding/Input</t>
   </si>
 </sst>
 </file>
@@ -907,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1099,7 @@
         <v>77</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
modbus temp channels control and reading of channels setup
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t>Range</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>Holding/Input</t>
+  </si>
+  <si>
+    <t>Channels control</t>
   </si>
 </sst>
 </file>
@@ -566,18 +569,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -598,21 +589,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -908,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M48"/>
+  <dimension ref="C2:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,15 +934,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="I2" s="24" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
+      <c r="I2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="24"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
@@ -1233,12 +1236,12 @@
       <c r="J26" s="13"/>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I27" s="41" t="s">
+      <c r="I27" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="43"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="49"/>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.3">
       <c r="K28" t="s">
@@ -1251,58 +1254,58 @@
       </c>
       <c r="D29" s="51"/>
       <c r="E29" s="52"/>
-      <c r="I29" s="25">
+      <c r="I29" s="21">
         <v>300</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K29" s="26">
+      <c r="K29" s="22">
         <v>4</v>
       </c>
-      <c r="L29" s="27" t="s">
+      <c r="L29" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C30" s="44">
+      <c r="C30" s="37">
         <v>0</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="46"/>
-      <c r="I30" s="28">
+      <c r="E30" s="39"/>
+      <c r="I30" s="24">
         <v>304</v>
       </c>
-      <c r="J30" s="29" t="s">
+      <c r="J30" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K30" s="29">
+      <c r="K30" s="25">
         <v>4</v>
       </c>
-      <c r="L30" s="30" t="s">
+      <c r="L30" s="26" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C31" s="44">
+      <c r="C31" s="37">
         <v>1</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="46"/>
-      <c r="I31" s="28">
+      <c r="E31" s="39"/>
+      <c r="I31" s="24">
         <v>308</v>
       </c>
-      <c r="J31" s="29" t="s">
+      <c r="J31" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="K31" s="29">
+      <c r="K31" s="25">
         <v>1</v>
       </c>
-      <c r="L31" s="30" t="s">
+      <c r="L31" s="26" t="s">
         <v>53</v>
       </c>
       <c r="M31" t="s">
@@ -1310,23 +1313,23 @@
       </c>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C32" s="44">
+      <c r="C32" s="37">
         <v>2</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="I32" s="28">
+      <c r="E32" s="39"/>
+      <c r="I32" s="24">
         <v>309</v>
       </c>
-      <c r="J32" s="29" t="s">
+      <c r="J32" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="K32" s="29">
+      <c r="K32" s="25">
         <v>1</v>
       </c>
-      <c r="L32" s="30" t="s">
+      <c r="L32" s="26" t="s">
         <v>53</v>
       </c>
       <c r="M32" t="s">
@@ -1334,246 +1337,262 @@
       </c>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C33" s="44">
+      <c r="C33" s="37">
         <v>3</v>
       </c>
-      <c r="D33" s="45" t="s">
+      <c r="D33" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="46"/>
-      <c r="I33" s="31">
+      <c r="E33" s="39"/>
+      <c r="I33" s="27">
         <v>310</v>
       </c>
-      <c r="J33" s="32" t="s">
+      <c r="J33" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="K33" s="32">
+      <c r="K33" s="28">
         <v>10</v>
       </c>
-      <c r="L33" s="33"/>
+      <c r="L33" s="29"/>
     </row>
     <row r="34" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C34" s="44">
+      <c r="C34" s="37">
         <v>4</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="46"/>
-      <c r="I34" s="31">
+      <c r="E34" s="39"/>
+      <c r="I34" s="27">
         <v>320</v>
       </c>
-      <c r="J34" s="32" t="s">
+      <c r="J34" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="K34" s="32">
+      <c r="K34" s="28">
         <v>10</v>
       </c>
-      <c r="L34" s="33"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C35" s="44">
+      <c r="C35" s="37">
         <v>5</v>
       </c>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="E35" s="46"/>
-      <c r="I35" s="34">
+      <c r="E35" s="39"/>
+      <c r="I35" s="30">
         <v>330</v>
       </c>
-      <c r="J35" s="35" t="s">
+      <c r="J35" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="K35" s="35">
+      <c r="K35" s="31">
         <v>10</v>
       </c>
-      <c r="L35" s="36"/>
+      <c r="L35" s="32"/>
     </row>
     <row r="36" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C36" s="44">
+      <c r="C36" s="37">
         <v>6</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="E36" s="46"/>
+      <c r="E36" s="39"/>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C37" s="44">
+      <c r="C37" s="37">
         <v>7</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="D37" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="46"/>
-      <c r="I37" s="25">
+      <c r="E37" s="39"/>
+      <c r="I37" s="28">
+        <v>340</v>
+      </c>
+      <c r="J37" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="K37" s="28">
+        <v>1</v>
+      </c>
+      <c r="L37" s="29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C38" s="37">
+        <v>8</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="39"/>
+    </row>
+    <row r="39" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C39" s="40">
+        <v>9</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="42"/>
+      <c r="I39" s="21">
         <v>350</v>
       </c>
-      <c r="J37" s="26" t="s">
+      <c r="J39" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="K37" s="26">
+      <c r="K39" s="22">
         <v>1</v>
       </c>
-      <c r="L37" s="27" t="s">
+      <c r="L39" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M39" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C38" s="44">
-        <v>8</v>
-      </c>
-      <c r="D38" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" s="46"/>
-      <c r="I38" s="28">
+    <row r="40" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I40" s="24">
         <v>351</v>
       </c>
-      <c r="J38" s="29" t="s">
+      <c r="J40" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="K38" s="29">
+      <c r="K40" s="25">
         <v>1</v>
       </c>
-      <c r="L38" s="30" t="s">
+      <c r="L40" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M40" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C39" s="47">
-        <v>9</v>
-      </c>
-      <c r="D39" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="49"/>
-      <c r="I39" s="28">
+    <row r="41" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I41" s="24">
         <v>352</v>
       </c>
-      <c r="J39" s="29" t="s">
+      <c r="J41" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="K39" s="29">
+      <c r="K41" s="25">
         <v>1</v>
       </c>
-      <c r="L39" s="30" t="s">
+      <c r="L41" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I40" s="31">
+    <row r="42" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I42" s="27">
         <v>353</v>
       </c>
-      <c r="J40" s="32" t="s">
+      <c r="J42" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="K40" s="32">
+      <c r="K42" s="28">
         <v>3</v>
       </c>
-      <c r="L40" s="33"/>
-    </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I41" s="31">
+      <c r="L42" s="29"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I43" s="27">
         <v>356</v>
       </c>
-      <c r="J41" s="32" t="s">
+      <c r="J43" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="K41" s="32">
+      <c r="K43" s="28">
         <v>3</v>
       </c>
-      <c r="L41" s="33"/>
-    </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I42" s="34">
+      <c r="L43" s="29"/>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I44" s="30">
         <v>359</v>
       </c>
-      <c r="J42" s="35" t="s">
+      <c r="J44" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="K42" s="35">
+      <c r="K44" s="31">
         <v>3</v>
       </c>
-      <c r="L42" s="36"/>
-    </row>
-    <row r="44" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I44" s="25">
+      <c r="L44" s="32"/>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I46" s="21">
         <v>400</v>
       </c>
-      <c r="J44" s="26" t="s">
+      <c r="J46" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="K44" s="26">
+      <c r="K46" s="22">
         <v>4</v>
       </c>
-      <c r="L44" s="27" t="s">
+      <c r="L46" s="23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I45" s="28">
+    <row r="47" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I47" s="24">
         <v>404</v>
       </c>
-      <c r="J45" s="29" t="s">
+      <c r="J47" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="K45" s="29">
+      <c r="K47" s="25">
         <v>1</v>
       </c>
-      <c r="L45" s="30" t="s">
+      <c r="L47" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M47" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I46" s="28">
+    <row r="48" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="I48" s="24">
         <v>405</v>
       </c>
-      <c r="J46" s="29" t="s">
+      <c r="J48" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="K46" s="29">
+      <c r="K48" s="25">
         <v>1</v>
       </c>
-      <c r="L46" s="30" t="s">
+      <c r="L48" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M48" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I47" s="37" t="s">
+    <row r="49" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I49" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="30"/>
-    </row>
-    <row r="48" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I48" s="38" t="s">
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="26"/>
+    </row>
+    <row r="50" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I50" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="J48" s="39" t="s">
+      <c r="J50" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="K48" s="39">
+      <c r="K50" s="35">
         <v>6</v>
       </c>
-      <c r="L48" s="40"/>
+      <c r="L50" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
eeprom const and modbus regmap
</commit_message>
<xml_diff>
--- a/docs/modbus_regmap.xlsx
+++ b/docs/modbus_regmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
   <si>
     <t>Range</t>
   </si>
@@ -306,6 +306,24 @@
   </si>
   <si>
     <t>bit0: channel1 … bit3: channel4 enable</t>
+  </si>
+  <si>
+    <t>500-516</t>
+  </si>
+  <si>
+    <t>executor setup</t>
+  </si>
+  <si>
+    <t>501-516</t>
+  </si>
+  <si>
+    <t>Executor</t>
+  </si>
+  <si>
+    <t>Config. b0 - triacs on=0 off=1</t>
+  </si>
+  <si>
+    <t>time switch on-&gt;off in 100ms</t>
   </si>
 </sst>
 </file>
@@ -600,6 +618,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -629,9 +650,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M50"/>
+  <dimension ref="C2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,15 +960,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="I2" s="45" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
+      <c r="I2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="45"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
@@ -1123,7 +1141,7 @@
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="52">
+      <c r="C13" s="42">
         <v>340</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -1174,6 +1192,15 @@
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="I16" s="11">
         <v>131</v>
       </c>
@@ -1253,12 +1280,12 @@
       <c r="J26" s="13"/>
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="I27" s="46" t="s">
+      <c r="I27" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="J27" s="47"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="49"/>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.3">
       <c r="K28" t="s">
@@ -1266,11 +1293,11 @@
       </c>
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="52"/>
       <c r="I29" s="21">
         <v>300</v>
       </c>
@@ -1625,6 +1652,39 @@
         <v>6</v>
       </c>
       <c r="L50" s="35"/>
+    </row>
+    <row r="52" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="J52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I53" s="21">
+        <v>500</v>
+      </c>
+      <c r="J53" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K53" s="22">
+        <v>1</v>
+      </c>
+      <c r="L53" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I54" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="J54" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="K54" s="34">
+        <v>2</v>
+      </c>
+      <c r="L54" s="35" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>